<commit_message>
postpone subboard step, add step to solder gate leds
</commit_message>
<xml_diff>
--- a/docs/gills/ksoloti_gills_bom.xlsx
+++ b/docs/gills/ksoloti_gills_bom.xlsx
@@ -408,10 +408,10 @@
     <t xml:space="preserve">SW1, SW2, SW3, SW4</t>
   </si>
   <si>
-    <t xml:space="preserve">TL1105_with_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Library:TL1105T_with_LED</t>
+    <t xml:space="preserve">TL1105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library:TL1105T</t>
   </si>
   <si>
     <t xml:space="preserve">Double Pole Single Throw (DPST) Switch  Momentary tact switch, 6*6mm. With 6.5mm diameter circular cap.</t>
@@ -522,7 +522,23 @@
     <t xml:space="preserve">HEAT1</t>
   </si>
   <si>
-    <t xml:space="preserve">Heatshrink, 3-4mm diameter, ca. 3cm length (optional)</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Isolation tape, or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Heatshrink, 3-4mm diameter, ca. 3cm length (optional)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Optional. For shielding LED1 and LED2 against light bleed from each other.</t>
@@ -611,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -652,6 +668,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -709,7 +730,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -734,6 +755,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -748,6 +773,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -837,9 +866,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2280600</xdr:colOff>
+      <xdr:colOff>2280240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>955080</xdr:rowOff>
+      <xdr:rowOff>954720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -853,7 +882,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13830480" y="5621400"/>
-          <a:ext cx="2275920" cy="1525680"/>
+          <a:ext cx="2275560" cy="1525320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -874,9 +903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3380400</xdr:colOff>
+      <xdr:colOff>3380040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>995040</xdr:rowOff>
+      <xdr:rowOff>994680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -890,7 +919,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17260560" y="5608080"/>
-          <a:ext cx="3376080" cy="1578960"/>
+          <a:ext cx="3375720" cy="1578600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1018,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1085,16 +1114,16 @@
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -1106,16 +1135,16 @@
       <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1129,16 +1158,16 @@
       <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -1150,16 +1179,16 @@
       <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
@@ -1171,16 +1200,16 @@
       <c r="C8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1194,16 +1223,16 @@
       <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1217,16 +1246,16 @@
       <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1240,16 +1269,16 @@
       <c r="C11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1263,16 +1292,16 @@
       <c r="C12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1286,16 +1315,16 @@
       <c r="C13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -1307,16 +1336,16 @@
       <c r="C14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -1328,16 +1357,16 @@
       <c r="C15" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1351,16 +1380,16 @@
       <c r="C16" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="9" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1374,16 +1403,16 @@
       <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1397,16 +1426,16 @@
       <c r="C18" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="124.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
@@ -1418,16 +1447,16 @@
       <c r="C19" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
@@ -1439,16 +1468,16 @@
       <c r="C20" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -1460,16 +1489,16 @@
       <c r="C21" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
@@ -1481,20 +1510,20 @@
       <c r="C22" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="23" s="9" customFormat="true" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="10" customFormat="true" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>112</v>
       </c>
@@ -1504,16 +1533,16 @@
       <c r="C23" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="6"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
@@ -1525,16 +1554,16 @@
       <c r="C24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
@@ -1546,16 +1575,16 @@
       <c r="C25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
@@ -1567,16 +1596,16 @@
       <c r="C26" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G26" s="6"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
@@ -1588,35 +1617,35 @@
       <c r="C27" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
@@ -1628,14 +1657,14 @@
       <c r="C29" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
@@ -1647,16 +1676,16 @@
       <c r="C30" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>139</v>
       </c>
@@ -1666,14 +1695,14 @@
       <c r="C31" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5" t="s">
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G31" s="6"/>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
@@ -1685,14 +1714,14 @@
       <c r="C32" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5" t="s">
+      <c r="E32" s="6"/>
+      <c r="F32" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G32" s="6"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
@@ -1704,14 +1733,14 @@
       <c r="C33" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="6"/>
+      <c r="F33" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G33" s="6"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
@@ -1723,14 +1752,14 @@
       <c r="C34" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G34" s="6"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
@@ -1742,14 +1771,14 @@
       <c r="C35" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
+      <c r="E35" s="6"/>
+      <c r="F35" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
@@ -1761,14 +1790,14 @@
       <c r="C36" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5" t="s">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="G36" s="6"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
@@ -1780,14 +1809,14 @@
       <c r="C37" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G37" s="6"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
@@ -1799,14 +1828,14 @@
       <c r="C38" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G38" s="6"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
@@ -1818,16 +1847,16 @@
       <c r="C39" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G39" s="6"/>
+      <c r="G39" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>